<commit_message>
edit all hello unit testts
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -64,16 +64,16 @@
     <t>element</t>
   </si>
   <si>
-    <t>-smile</t>
-  </si>
-  <si>
     <t>Jenkins T5</t>
   </si>
   <si>
-    <t>-noExistElement</t>
-  </si>
-  <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>smile</t>
+  </si>
+  <si>
+    <t>noExistElement</t>
   </si>
 </sst>
 </file>
@@ -108,7 +108,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,10 +156,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +469,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +495,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -506,80 +512,86 @@
         <v>4</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="12">
+        <v>17</v>
+      </c>
+      <c r="E2" s="9">
         <v>43846</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12">
+        <v>17</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
add UT for new feature: ("I save the value of '(.*)-(.*)' in '(.*)' column of data output provider.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Résultat</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>noExistElement</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,11 +480,11 @@
     <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -498,10 +501,13 @@
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -517,10 +523,11 @@
       <c r="E2" s="9">
         <v>43846</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="9"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -534,12 +541,13 @@
         <v>17</v>
       </c>
       <c r="E3" s="11"/>
-      <c r="F3" s="12">
+      <c r="F3" s="11"/>
+      <c r="G3" s="12">
         <v>23</v>
       </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -553,12 +561,13 @@
         <v>17</v>
       </c>
       <c r="E4" s="11"/>
-      <c r="F4" s="12">
+      <c r="F4" s="11"/>
+      <c r="G4" s="12">
         <v>17</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -572,10 +581,11 @@
         <v>17</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="8"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -589,47 +599,48 @@
         <v>18</v>
       </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="12">
+      <c r="F6" s="11"/>
+      <c r="G6" s="12">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>

</xml_diff>

<commit_message>
update unit tests for coverage
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Résultat</t>
   </si>
@@ -481,7 +481,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,9 +637,7 @@
       <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>

</xml_diff>

<commit_message>
update unit tests for quality coverage
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Résultat</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Jenkins T8</t>
+  </si>
+  <si>
+    <t>element2</t>
   </si>
 </sst>
 </file>
@@ -478,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,11 +492,11 @@
     <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -506,17 +509,20 @@
       <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -529,14 +535,17 @@
       <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="9">
         <v>43846</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="9"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -549,14 +558,17 @@
       <c r="D3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="F3" s="11"/>
-      <c r="G3" s="12">
+      <c r="G3" s="11"/>
+      <c r="H3" s="12">
         <v>24</v>
       </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -569,14 +581,17 @@
       <c r="D4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="11"/>
-      <c r="G4" s="12">
+      <c r="G4" s="11"/>
+      <c r="H4" s="12">
         <v>18</v>
       </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -589,12 +604,15 @@
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F5" s="8"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="8"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -607,13 +625,16 @@
       <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="12">
+      <c r="G6" s="11"/>
+      <c r="H6" s="12">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -624,28 +645,34 @@
       <c r="D7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="12">
+      <c r="G7" s="11"/>
+      <c r="H7" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="12">
+      <c r="G8" s="11"/>
+      <c r="H8" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
@@ -656,37 +683,40 @@
       <c r="D9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="F9" s="11"/>
-      <c r="G9" s="12">
+      <c r="G9" s="11"/>
+      <c r="H9" s="12">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>

</xml_diff>

<commit_message>
use data from Context (after a save) fixed issue to html alert fixed issue to clickOnByJs for IE add new unit tests clean code
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -484,7 +484,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="12">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New feature: file upload
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14670" windowHeight="5745"/>
@@ -190,6 +190,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -237,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,7 +275,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -484,7 +487,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +567,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="12">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -587,7 +590,7 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="12">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -631,7 +634,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="12">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -689,7 +692,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add unit test on video capture (French part)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14670" windowHeight="5745"/>
@@ -240,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,7 +275,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -487,7 +487,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +567,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="12">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -590,7 +590,7 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -634,7 +634,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="12">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update counter for new step (new unit test)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -489,7 +489,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="9">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="9">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix all counter in data
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -489,7 +489,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="9">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="9">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix CI (future date in 2050)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\POC\NoraUi\src\test\resources\data\in\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="NoraUi-bonjour" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NoraUi-bonjour" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="Motifs" vbProcedure="false">#REF!</definedName>
+    <definedName name="Motifs">#REF!</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,88 +29,86 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
-    <t xml:space="preserve">auteur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">codepostal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">élément</t>
-  </si>
-  <si>
-    <t xml:space="preserve">élément2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">titre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résultat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins T1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rennes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins T2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins T3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lorient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins T4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins T5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noExistElement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins T6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins T7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins T8</t>
+    <t>auteur</t>
+  </si>
+  <si>
+    <t>codepostal</t>
+  </si>
+  <si>
+    <t>ville</t>
+  </si>
+  <si>
+    <t>élément</t>
+  </si>
+  <si>
+    <t>élément2</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>titre</t>
+  </si>
+  <si>
+    <t>Résultat</t>
+  </si>
+  <si>
+    <t>Jenkins T1</t>
+  </si>
+  <si>
+    <t>35000</t>
+  </si>
+  <si>
+    <t>Rennes</t>
+  </si>
+  <si>
+    <t>smile</t>
+  </si>
+  <si>
+    <t>Jenkins T2</t>
+  </si>
+  <si>
+    <t>75000</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Jenkins T3</t>
+  </si>
+  <si>
+    <t>56100</t>
+  </si>
+  <si>
+    <t>Lorient</t>
+  </si>
+  <si>
+    <t>Jenkins T4</t>
+  </si>
+  <si>
+    <t>Jenkins T5</t>
+  </si>
+  <si>
+    <t>noExistElement</t>
+  </si>
+  <si>
+    <t>Jenkins T6</t>
+  </si>
+  <si>
+    <t>Jenkins T7</t>
+  </si>
+  <si>
+    <t>Jenkins T8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-40C]DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-40C]dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -115,22 +117,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -177,7 +164,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -185,85 +172,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -322,31 +251,303 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.28"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="4" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -372,7 +573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -388,14 +589,14 @@
       <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="n">
-        <v>43846</v>
+      <c r="F2" s="5">
+        <v>54804</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -413,12 +614,12 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="9" t="n">
+      <c r="H3" s="9">
         <v>31</v>
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -436,12 +637,12 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="9" t="n">
+      <c r="H4" s="9">
         <v>25</v>
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -462,7 +663,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
@@ -480,11 +681,11 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="9" t="n">
+      <c r="H6" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -500,11 +701,11 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="9" t="n">
+      <c r="H7" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
@@ -518,11 +719,11 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="9" t="n">
+      <c r="H8" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
@@ -538,137 +739,132 @@
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="9" t="n">
+      <c r="H9" s="9">
         <v>58</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ChainableWaits + step numbers + colors + rework driver restart + PageElement & Page cucumber param
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/bonjour.xlsx
+++ b/src/test/resources/data/in/bonjour.xlsx
@@ -103,7 +103,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-40C]DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="[$-40C]dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="7">
@@ -210,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,10 +236,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -335,10 +331,10 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
@@ -389,57 +385,55 @@
         <v>11</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>43846</v>
+        <v>54804</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9" t="n">
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="n">
         <v>31</v>
       </c>
-      <c r="I3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9" t="n">
+      <c r="D4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
@@ -460,85 +454,84 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9" t="n">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9" t="n">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9" t="n">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9" t="n">
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8" t="n">
         <v>58</v>
       </c>
     </row>

</xml_diff>